<commit_message>
Dummy Data now is added to Excel file
</commit_message>
<xml_diff>
--- a/Excel/Manipulator.xlsx
+++ b/Excel/Manipulator.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>Business Name</t>
   </si>
@@ -39,6 +39,54 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Fernando's Laboratory</t>
+  </si>
+  <si>
+    <t>Lab</t>
+  </si>
+  <si>
+    <t>7 W Lane, Central NY NY 11723</t>
+  </si>
+  <si>
+    <t>wwww.tcgdex.net</t>
+  </si>
+  <si>
+    <t>fernhean@hotmail.nw</t>
+  </si>
+  <si>
+    <t>123-456-7890</t>
+  </si>
+  <si>
+    <t>312-312-4212</t>
+  </si>
+  <si>
+    <t>My lab is full of enourmous surprises</t>
+  </si>
+  <si>
+    <t>Tiffy's Bunnies</t>
+  </si>
+  <si>
+    <t>Animal Care</t>
+  </si>
+  <si>
+    <t>Earth</t>
+  </si>
+  <si>
+    <t>tiffysbunnies.com</t>
+  </si>
+  <si>
+    <t>tiffy23@aol.321</t>
+  </si>
+  <si>
+    <t>653-123-4632</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>The most epic bunnies in existance!</t>
   </si>
 </sst>
 </file>
@@ -388,8 +436,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="50" customWidth="true" style="0"/>
-    <col min="8" max="8" width="150" customWidth="true" style="0"/>
+    <col min="1" max="1" width="30" customWidth="true" style="0"/>
+    <col min="2" max="2" width="15" customWidth="true" style="0"/>
+    <col min="3" max="3" width="40" customWidth="true" style="0"/>
+    <col min="4" max="4" width="25" customWidth="true" style="0"/>
+    <col min="5" max="5" width="25" customWidth="true" style="0"/>
+    <col min="6" max="6" width="15" customWidth="true" style="0"/>
+    <col min="7" max="7" width="15" customWidth="true" style="0"/>
+    <col min="8" max="8" width="80" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -416,6 +470,58 @@
       </c>
       <c r="H1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8">

</xml_diff>